<commit_message>
Created traps and target
</commit_message>
<xml_diff>
--- a/Календарный план.xlsx
+++ b/Календарный план.xlsx
@@ -45,9 +45,6 @@
     <t>Действие</t>
   </si>
   <si>
-    <t>Генерация лабиринта</t>
-  </si>
-  <si>
     <t>Кнопка перегенерации лабиринта</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>Разные уровни (разные спрайты лабиринтов)</t>
   </si>
   <si>
-    <t>Переход на следий уровень</t>
-  </si>
-  <si>
     <t>Этап 1</t>
   </si>
   <si>
@@ -103,6 +97,12 @@
   </si>
   <si>
     <t>10.04 - 12.04</t>
+  </si>
+  <si>
+    <t>Переход на следующий уровень</t>
+  </si>
+  <si>
+    <t>Процедурная генерация лабиринта</t>
   </si>
 </sst>
 </file>
@@ -616,40 +616,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -669,17 +642,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -691,9 +655,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -708,6 +669,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1003,7 +1003,7 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A14" sqref="A14:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1020,130 +1020,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="50" t="s">
+      <c r="B1" s="50"/>
+      <c r="C1" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="38" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="48"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
+      <c r="A2" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="35"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="23" t="s">
+      <c r="A3" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="13"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="44"/>
+      <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="19"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="11" t="s">
-        <v>15</v>
-      </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="53"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="11"/>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
+      <c r="J4" s="8"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>14</v>
+      <c r="A5" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="10"/>
-      <c r="L5" s="52"/>
+      <c r="J5" s="7"/>
+      <c r="L5" s="39"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="52"/>
+      <c r="N5" s="39"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="11"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="52"/>
+      <c r="J6" s="8"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="39"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>14</v>
+      <c r="A7" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="1"/>
@@ -1152,51 +1152,51 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="10"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52"/>
+      <c r="J7" s="7"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="11" t="s">
-        <v>15</v>
+      <c r="A8" s="44"/>
+      <c r="B8" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="41"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="11"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="52"/>
-      <c r="N8" s="52"/>
+      <c r="J8" s="8"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>14</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="41"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="52"/>
+      <c r="J9" s="29"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="39"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="11" t="s">
-        <v>15</v>
+      <c r="A10" s="44"/>
+      <c r="B10" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="3"/>
@@ -1205,78 +1205,78 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="11"/>
-      <c r="L10" s="52"/>
-      <c r="M10" s="52"/>
-      <c r="N10" s="52"/>
+      <c r="J10" s="8"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>14</v>
+      <c r="A11" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C11" s="6"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="10"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="52"/>
+      <c r="J11" s="7"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
     </row>
     <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="30"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="21"/>
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="33"/>
+      <c r="A13" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="54"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="24"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="10" t="s">
+      <c r="A14" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="44"/>
+      <c r="B15" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="19"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="11" t="s">
-        <v>15</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="3"/>
@@ -1285,14 +1285,14 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="11"/>
+      <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>14</v>
+      <c r="A16" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="2"/>
@@ -1301,12 +1301,12 @@
       <c r="G16" s="1"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="10"/>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
-      <c r="B17" s="11" t="s">
-        <v>15</v>
+      <c r="A17" s="44"/>
+      <c r="B17" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="3"/>
@@ -1315,14 +1315,14 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="11"/>
+      <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>14</v>
+      <c r="A18" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="2"/>
@@ -1331,12 +1331,12 @@
       <c r="G18" s="1"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="10"/>
+      <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
-      <c r="B19" s="11" t="s">
-        <v>15</v>
+      <c r="A19" s="44"/>
+      <c r="B19" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="3"/>
@@ -1345,14 +1345,14 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="11"/>
+      <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>14</v>
+      <c r="A20" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="2"/>
@@ -1361,56 +1361,56 @@
       <c r="G20" s="1"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="10"/>
+      <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="30"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="21"/>
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="54"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="24"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="33"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="22"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="44"/>
+      <c r="B24" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="31"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
-      <c r="B24" s="11" t="s">
-        <v>15</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="3"/>
@@ -1419,14 +1419,14 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
-      <c r="J24" s="26"/>
+      <c r="J24" s="17"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>14</v>
+      <c r="A25" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="2"/>
@@ -1435,12 +1435,12 @@
       <c r="G25" s="6"/>
       <c r="H25" s="4"/>
       <c r="I25" s="6"/>
-      <c r="J25" s="25"/>
+      <c r="J25" s="16"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
-      <c r="B26" s="11" t="s">
-        <v>15</v>
+      <c r="A26" s="44"/>
+      <c r="B26" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="3"/>
@@ -1449,14 +1449,14 @@
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
-      <c r="J26" s="26"/>
+      <c r="J26" s="17"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>14</v>
+      <c r="A27" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="2"/>
@@ -1465,12 +1465,12 @@
       <c r="G27" s="6"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
-      <c r="J27" s="25"/>
+      <c r="J27" s="16"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="11" t="s">
-        <v>15</v>
+      <c r="A28" s="44"/>
+      <c r="B28" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="3"/>
@@ -1479,14 +1479,14 @@
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
-      <c r="J28" s="26"/>
+      <c r="J28" s="17"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>14</v>
+      <c r="A29" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="2"/>
@@ -1495,68 +1495,66 @@
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
-      <c r="J29" s="25"/>
+      <c r="J29" s="16"/>
     </row>
     <row r="30" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="12"/>
-      <c r="B30" s="13" t="s">
+      <c r="A30" s="45"/>
+      <c r="B30" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="10"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="25"/>
+    </row>
+    <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="47"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="24"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="34"/>
-    </row>
-    <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="36"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="33"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="11"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="26"/>
+    </row>
+    <row r="33" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="43"/>
+      <c r="B33" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="17"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="35"/>
-    </row>
-    <row r="33" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="15"/>
-      <c r="B33" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="27"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="28"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A31:B31"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A13:B13"/>
@@ -1574,6 +1572,8 @@
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A31:B31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>